<commit_message>
Implement toolbox talks fetching and attendee listing functionality
</commit_message>
<xml_diff>
--- a/Crew_Sheet.xlsx
+++ b/Crew_Sheet.xlsx
@@ -35,6 +35,15 @@
     <t>Equip</t>
   </si>
   <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
     <t>Th</t>
   </si>
   <si>
@@ -42,15 +51,6 @@
   </si>
   <si>
     <t>S</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>W</t>
   </si>
   <si>
     <t>12/14</t>
@@ -427,22 +427,22 @@
     <row r="3"/>
     <row r="4">
       <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
random changes broken state
</commit_message>
<xml_diff>
--- a/Crew_Sheet.xlsx
+++ b/Crew_Sheet.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>TIMESHEET REVIEW / RECAP</t>
   </si>
@@ -23,6 +22,9 @@
     <t>Saturday, December 20, 2025</t>
   </si>
   <si>
+    <t>Equip</t>
+  </si>
+  <si>
     <t>Last Name</t>
   </si>
   <si>
@@ -32,46 +34,40 @@
     <t>Class</t>
   </si>
   <si>
-    <t>Equip</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
+    <t>12/15</t>
+  </si>
+  <si>
     <t>T</t>
   </si>
   <si>
+    <t>12/16</t>
+  </si>
+  <si>
     <t>W</t>
   </si>
   <si>
+    <t>12/17</t>
+  </si>
+  <si>
     <t>Th</t>
   </si>
   <si>
+    <t>12/18</t>
+  </si>
+  <si>
     <t>F</t>
   </si>
   <si>
+    <t>12/19</t>
+  </si>
+  <si>
     <t>S</t>
   </si>
   <si>
-    <t>12/14</t>
-  </si>
-  <si>
-    <t>12/15</t>
-  </si>
-  <si>
-    <t>12/16</t>
-  </si>
-  <si>
-    <t>12/17</t>
-  </si>
-  <si>
-    <t>12/18</t>
-  </si>
-  <si>
-    <t>12/19</t>
-  </si>
-  <si>
-    <t>This is on Sheet 2!</t>
+    <t>12/20</t>
   </si>
 </sst>
 </file>
@@ -81,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dddd, mmmm dd, yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -104,6 +100,12 @@
       <family val="2"/>
       <color/>
       <sz val="14"/>
+    </font>
+    <font>
+      <family val="2"/>
+      <b val="1"/>
+      <color/>
+      <u val="single"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false">
       <alignment/>
@@ -140,6 +142,9 @@
       <alignment/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="false">
       <alignment/>
     </xf>
   </cellXfs>
@@ -414,9 +419,13 @@
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="true" max="1" min="1" width="30"/>
+    <col customWidth="true" max="4" min="2" width="15"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -430,68 +439,51 @@
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1"/>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>